<commit_message>
updated for sprint 3
</commit_message>
<xml_diff>
--- a/documentation/Req_SSTP.xlsx
+++ b/documentation/Req_SSTP.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="18195" windowHeight="10800" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="18195" windowHeight="10800"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,8 +18,8 @@
   </definedNames>
   <calcPr calcId="145621"/>
   <customWorkbookViews>
+    <customWorkbookView name="Emna Mokaddem - Personal View" guid="{62558FE4-8837-4E09-B150-242C582E08A1}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1262" windowHeight="647" activeSheetId="1"/>
     <customWorkbookView name="Lavignotte Fabien - Personal View" guid="{DA65F8B0-9E28-4694-AD16-567217749021}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1676" windowHeight="765" activeSheetId="2"/>
-    <customWorkbookView name="Emna Mokaddem - Personal View" guid="{62558FE4-8837-4E09-B150-242C582E08A1}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1262" windowHeight="647" activeSheetId="1"/>
   </customWorkbookViews>
 </workbook>
 </file>
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="664" uniqueCount="419">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="672" uniqueCount="427">
   <si>
     <t>SSRD-WC Requirement ID</t>
   </si>
@@ -1318,6 +1318,30 @@
   <si>
     <t xml:space="preserve">ngEO-SUB-001-WEBC-DES ngEO-SUB-002-WEBC-DES  ngEO-SUB-800-WEBC-TVA
 </t>
+  </si>
+  <si>
+    <t> NGEO-WEBC-VTC-0150  NGEO-WEBC-VTC-0151</t>
+  </si>
+  <si>
+    <t> NGEO-WEBC-VTC-0120 NGEO-WEBC-VTC-0121 NGEO-WEBC-VTC-0122</t>
+  </si>
+  <si>
+    <t>NGEO-WEBC-VTC-0030 NGEO-WEBC-VTC-0110 NGEO-WEBC-VTC-0150</t>
+  </si>
+  <si>
+    <t>NGEO-WEBC-VTC-0140</t>
+  </si>
+  <si>
+    <t>NGEO-WEBC-VTC-0150 NGEO-WEBC-VTC-0151</t>
+  </si>
+  <si>
+    <t>NGEO-WEBC-VTC-0110 NGEO-WEBC-VTC-0120</t>
+  </si>
+  <si>
+    <t>NGEO-WEBC-VTC-0120 NGEO-WEBC-VTC-0121 NGEO-WEBC-VTC-0122</t>
+  </si>
+  <si>
+    <t>NGEO-WEBC-VTC-0130 NGEO-WEBC-VTC-0131 NGEO-WEBC-VTC-0140</t>
   </si>
 </sst>
 </file>
@@ -1486,7 +1510,7 @@
 </file>
 
 <file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
-<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{B5AB8769-C77D-4186-8BBA-EFC275CDF7FF}" diskRevisions="1" revisionId="10" version="4">
+<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{1A1410C6-C537-4E1D-9FAE-AB370FA54851}" diskRevisions="1" revisionId="22" version="12">
   <header guid="{4F90D1E1-98D7-43D2-BD00-631CFD24DD58}" dateTime="2012-11-30T15:11:14" maxSheetId="4" userName="Emna Mokaddem" r:id="rId1">
     <sheetIdMap count="3">
       <sheetId val="1"/>
@@ -1515,11 +1539,153 @@
       <sheetId val="3"/>
     </sheetIdMap>
   </header>
+  <header guid="{755277DC-E97B-44D5-BDFA-8A643EF26744}" dateTime="2012-12-19T15:21:11" maxSheetId="4" userName="Emna Mokaddem" r:id="rId5" minRId="11">
+    <sheetIdMap count="3">
+      <sheetId val="1"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{090B22D8-62F3-4667-B940-E633408096E7}" dateTime="2012-12-19T15:42:52" maxSheetId="4" userName="Emna Mokaddem" r:id="rId6" minRId="12">
+    <sheetIdMap count="3">
+      <sheetId val="1"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{98295BD7-6E99-474A-95C7-7460302F5152}" dateTime="2012-12-19T15:44:57" maxSheetId="4" userName="Emna Mokaddem" r:id="rId7" minRId="13" maxRId="14">
+    <sheetIdMap count="3">
+      <sheetId val="1"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{C77DDF6D-9750-4841-AE49-04C555B6F241}" dateTime="2012-12-19T15:48:32" maxSheetId="4" userName="Emna Mokaddem" r:id="rId8" minRId="15">
+    <sheetIdMap count="3">
+      <sheetId val="1"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{DD11029A-8C53-4272-B2AE-E362243EAF56}" dateTime="2012-12-19T15:49:13" maxSheetId="4" userName="Emna Mokaddem" r:id="rId9" minRId="16">
+    <sheetIdMap count="3">
+      <sheetId val="1"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{AB6DB1AF-83EC-4282-B66A-2D8005598C42}" dateTime="2012-12-19T15:52:58" maxSheetId="4" userName="Emna Mokaddem" r:id="rId10" minRId="17" maxRId="19">
+    <sheetIdMap count="3">
+      <sheetId val="1"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{6260F9B6-0FE3-4387-8F40-3014E06E02D1}" dateTime="2012-12-19T15:54:16" maxSheetId="4" userName="Emna Mokaddem" r:id="rId11" minRId="20">
+    <sheetIdMap count="3">
+      <sheetId val="1"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{1A1410C6-C537-4E1D-9FAE-AB370FA54851}" dateTime="2012-12-19T15:56:18" maxSheetId="4" userName="Emna Mokaddem" r:id="rId12" minRId="21" maxRId="22">
+    <sheetIdMap count="3">
+      <sheetId val="1"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+    </sheetIdMap>
+  </header>
 </headers>
 </file>
 
 <file path=xl/revisions/revisionLog1.xml><?xml version="1.0" encoding="utf-8"?>
 <revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac"/>
+</file>
+
+<file path=xl/revisions/revisionLog10.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rfmt sheetId="1" xfDxf="1" sqref="D94" start="0" length="0">
+    <dxf>
+      <font>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <name val="Times New Roman"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="justify" vertical="center" wrapText="1" readingOrder="0"/>
+      <border outline="0">
+        <right style="medium">
+          <color rgb="FF808080"/>
+        </right>
+        <bottom style="medium">
+          <color rgb="FF808080"/>
+        </bottom>
+      </border>
+    </dxf>
+  </rfmt>
+  <rcc rId="17" sId="1">
+    <nc r="D94" t="inlineStr">
+      <is>
+        <t>NGEO-WEBC-VTC-0150 NGEO-WEBC-VTC-0151</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="18" sId="1">
+    <oc r="D95" t="inlineStr">
+      <is>
+        <t>NGEO-WEBC-VTC-0110</t>
+      </is>
+    </oc>
+    <nc r="D95" t="inlineStr">
+      <is>
+        <t>NGEO-WEBC-VTC-0110 NGEO-WEBC-VTC-0120</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="19" sId="1">
+    <oc r="D100" t="inlineStr">
+      <is>
+        <t>NGEO-WEBC-VTC-0120</t>
+      </is>
+    </oc>
+    <nc r="D100" t="inlineStr">
+      <is>
+        <t>NGEO-WEBC-VTC-0120 NGEO-WEBC-VTC-0121 NGEO-WEBC-VTC-0122</t>
+      </is>
+    </nc>
+  </rcc>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog11.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="20" sId="1">
+    <nc r="D103" t="inlineStr">
+      <is>
+        <t>NGEO-WEBC-VTC-0140</t>
+      </is>
+    </nc>
+  </rcc>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog12.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="21" sId="1">
+    <nc r="D104" t="inlineStr">
+      <is>
+        <t>NGEO-WEBC-VTC-0130 NGEO-WEBC-VTC-0131 NGEO-WEBC-VTC-0140</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="22" sId="1">
+    <nc r="D107" t="inlineStr">
+      <is>
+        <t>NGEO-WEBC-VTC-0130 NGEO-WEBC-VTC-0131 NGEO-WEBC-VTC-0140</t>
+      </is>
+    </nc>
+  </rcc>
+</revisions>
 </file>
 
 <file path=xl/revisions/revisionLog2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1720,7 +1886,122 @@
 </revisions>
 </file>
 
-<file path=xl/revisions/userNames.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/revisions/revisionLog5.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="11" sId="1">
+    <nc r="D26" t="inlineStr">
+      <is>
+        <t> NGEO-WEBC-VTC-0150  NGEO-WEBC-VTC-0151</t>
+      </is>
+    </nc>
+  </rcc>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog6.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="12" sId="1">
+    <nc r="D36" t="inlineStr">
+      <is>
+        <t> NGEO-WEBC-VTC-0120  NGEO-WEBC-VTC-0121 NGEO-WEBC-VTC-0122</t>
+      </is>
+    </nc>
+  </rcc>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog7.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="13" sId="1">
+    <oc r="D36" t="inlineStr">
+      <is>
+        <t> NGEO-WEBC-VTC-0120  NGEO-WEBC-VTC-0121 NGEO-WEBC-VTC-0122</t>
+      </is>
+    </oc>
+    <nc r="D36" t="inlineStr">
+      <is>
+        <t> NGEO-WEBC-VTC-0120 NGEO-WEBC-VTC-0121 NGEO-WEBC-VTC-0122</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="14" sId="1">
+    <oc r="D44" t="inlineStr">
+      <is>
+        <t>NGEO-WEBC-VTC-0030</t>
+      </is>
+    </oc>
+    <nc r="D44" t="inlineStr">
+      <is>
+        <t>NGEO-WEBC-VTC-0030 NGEO-WEBC-VTC-0110 NGEO-WEBC-VTC-0150</t>
+      </is>
+    </nc>
+  </rcc>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog8.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rfmt sheetId="1" xfDxf="1" sqref="D93" start="0" length="0">
+    <dxf>
+      <font>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <name val="Times New Roman"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="justify" vertical="center" wrapText="1" readingOrder="0"/>
+      <border outline="0">
+        <right style="medium">
+          <color rgb="FF808080"/>
+        </right>
+        <bottom style="medium">
+          <color rgb="FF808080"/>
+        </bottom>
+      </border>
+    </dxf>
+  </rfmt>
+  <rcc rId="15" sId="1">
+    <nc r="D93" t="inlineStr">
+      <is>
+        <t>NGEO-WEBC-VTC-0140</t>
+      </is>
+    </nc>
+  </rcc>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog9.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rfmt sheetId="1" xfDxf="1" sqref="D101" start="0" length="0">
+    <dxf>
+      <font>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <name val="Times New Roman"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="justify" vertical="center" wrapText="1" readingOrder="0"/>
+      <border outline="0">
+        <right style="medium">
+          <color rgb="FF808080"/>
+        </right>
+        <bottom style="medium">
+          <color rgb="FF808080"/>
+        </bottom>
+      </border>
+    </dxf>
+  </rfmt>
+  <rcc rId="16" sId="1">
+    <nc r="D101" t="inlineStr">
+      <is>
+        <t>NGEO-WEBC-VTC-0140</t>
+      </is>
+    </nc>
+  </rcc>
+</revisions>
+</file>
+
+<file path=xl/revisions/userNames1.xml><?xml version="1.0" encoding="utf-8"?>
 <users xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" count="2">
   <userInfo guid="{A8C1A900-A0EB-4515-8E78-8138C0C42F21}" name="Emna Mokaddem" id="-2083828105" dateTime="2012-11-30T15:11:14"/>
   <userInfo guid="{BFC4EE2A-90DF-4511-9F1D-C131A45F9081}" name="Emna Mokaddem" id="-2083842149" dateTime="2012-12-10T10:19:06"/>
@@ -2016,8 +2297,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D191"/>
   <sheetViews>
-    <sheetView topLeftCell="A112" workbookViewId="0">
-      <selection activeCell="A141" sqref="A141"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="C45" sqref="C45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2358,7 +2639,9 @@
       <c r="C26" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="D26" s="6"/>
+      <c r="D26" s="6" t="s">
+        <v>419</v>
+      </c>
     </row>
     <row r="27" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="5" t="s">
@@ -2468,7 +2751,7 @@
       </c>
       <c r="D35" s="6"/>
     </row>
-    <row r="36" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="5" t="s">
         <v>78</v>
       </c>
@@ -2478,7 +2761,9 @@
       <c r="C36" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="D36" s="6"/>
+      <c r="D36" s="6" t="s">
+        <v>420</v>
+      </c>
     </row>
     <row r="37" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="5" t="s">
@@ -2564,7 +2849,7 @@
       </c>
       <c r="D43" s="6"/>
     </row>
-    <row r="44" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:4" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="5" t="s">
         <v>94</v>
       </c>
@@ -2575,7 +2860,7 @@
         <v>50</v>
       </c>
       <c r="D44" s="6" t="s">
-        <v>138</v>
+        <v>421</v>
       </c>
     </row>
     <row r="45" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3200,7 +3485,9 @@
       <c r="C93" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="D93" s="6"/>
+      <c r="D93" s="6" t="s">
+        <v>422</v>
+      </c>
     </row>
     <row r="94" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A94" s="5" t="s">
@@ -3212,7 +3499,9 @@
       <c r="C94" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="D94" s="6"/>
+      <c r="D94" s="6" t="s">
+        <v>423</v>
+      </c>
     </row>
     <row r="95" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A95" s="5" t="s">
@@ -3225,7 +3514,7 @@
         <v>50</v>
       </c>
       <c r="D95" s="6" t="s">
-        <v>416</v>
+        <v>424</v>
       </c>
     </row>
     <row r="96" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3280,7 +3569,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="100" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:4" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A100" s="5" t="s">
         <v>202</v>
       </c>
@@ -3291,7 +3580,7 @@
         <v>50</v>
       </c>
       <c r="D100" s="6" t="s">
-        <v>417</v>
+        <v>425</v>
       </c>
     </row>
     <row r="101" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3304,7 +3593,9 @@
       <c r="C101" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="D101" s="6"/>
+      <c r="D101" s="6" t="s">
+        <v>422</v>
+      </c>
     </row>
     <row r="102" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A102" s="5" t="s">
@@ -3328,9 +3619,11 @@
       <c r="C103" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="D103" s="6"/>
-    </row>
-    <row r="104" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D103" s="6" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A104" s="5" t="s">
         <v>210</v>
       </c>
@@ -3340,7 +3633,9 @@
       <c r="C104" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="D104" s="6"/>
+      <c r="D104" s="6" t="s">
+        <v>426</v>
+      </c>
     </row>
     <row r="105" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A105" s="5" t="s">
@@ -3370,7 +3665,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="107" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:4" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A107" s="5" t="s">
         <v>216</v>
       </c>
@@ -3380,7 +3675,9 @@
       <c r="C107" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="D107" s="6"/>
+      <c r="D107" s="6" t="s">
+        <v>426</v>
+      </c>
     </row>
     <row r="108" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A108" s="5" t="s">
@@ -4397,14 +4694,14 @@
   </sheetData>
   <autoFilter ref="A1:D191"/>
   <customSheetViews>
-    <customSheetView guid="{DA65F8B0-9E28-4694-AD16-567217749021}" showAutoFilter="1" topLeftCell="A112">
-      <selection activeCell="A141" sqref="A141"/>
+    <customSheetView guid="{62558FE4-8837-4E09-B150-242C582E08A1}" showAutoFilter="1" topLeftCell="A4">
+      <selection activeCell="D10" sqref="D10"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
       <autoFilter ref="A1:D191"/>
     </customSheetView>
-    <customSheetView guid="{62558FE4-8837-4E09-B150-242C582E08A1}" showAutoFilter="1" topLeftCell="A4">
-      <selection activeCell="D10" sqref="D10"/>
+    <customSheetView guid="{DA65F8B0-9E28-4694-AD16-567217749021}" showAutoFilter="1" topLeftCell="A112">
+      <selection activeCell="A141" sqref="A141"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
       <autoFilter ref="A1:D191"/>
@@ -4420,8 +4717,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4532,12 +4829,12 @@
     </row>
   </sheetData>
   <customSheetViews>
+    <customSheetView guid="{62558FE4-8837-4E09-B150-242C582E08A1}">
+      <selection activeCell="C29" sqref="C29"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+    </customSheetView>
     <customSheetView guid="{DA65F8B0-9E28-4694-AD16-567217749021}">
       <selection activeCell="E8" sqref="E8"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-    </customSheetView>
-    <customSheetView guid="{62558FE4-8837-4E09-B150-242C582E08A1}">
-      <selection activeCell="C29" sqref="C29"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
   </customSheetViews>
@@ -4661,11 +4958,11 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{DA65F8B0-9E28-4694-AD16-567217749021}">
+    <customSheetView guid="{62558FE4-8837-4E09-B150-242C582E08A1}">
       <selection activeCell="C16" sqref="C16"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
-    <customSheetView guid="{62558FE4-8837-4E09-B150-242C582E08A1}">
+    <customSheetView guid="{DA65F8B0-9E28-4694-AD16-567217749021}">
       <selection activeCell="C16" sqref="C16"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>

</xml_diff>

<commit_message>
update VTP ids 121 to 125 and 122 to 126
</commit_message>
<xml_diff>
--- a/documentation/Req_SSTP.xlsx
+++ b/documentation/Req_SSTP.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="165" windowWidth="18195" windowHeight="10740" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="165" windowWidth="18195" windowHeight="10740"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,8 +18,8 @@
   </definedNames>
   <calcPr calcId="145621"/>
   <customWorkbookViews>
+    <customWorkbookView name="Emna Mokaddem - Personal View" guid="{62558FE4-8837-4E09-B150-242C582E08A1}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1262" windowHeight="647" activeSheetId="1"/>
     <customWorkbookView name="Lavignotte Fabien - Personal View" guid="{DA65F8B0-9E28-4694-AD16-567217749021}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1676" windowHeight="765" activeSheetId="2"/>
-    <customWorkbookView name="Emna Mokaddem - Personal View" guid="{62558FE4-8837-4E09-B150-242C582E08A1}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1262" windowHeight="647" activeSheetId="1"/>
   </customWorkbookViews>
 </workbook>
 </file>
@@ -1292,9 +1292,6 @@
     <t>NGEO-WEBC-VTC-0120</t>
   </si>
   <si>
-    <t> NGEO-WEBC-VTC-0120 NGEO-WEBC-VTC-0121 NGEO-WEBC-VTC-0122</t>
-  </si>
-  <si>
     <t>NGEO-WEBC-VTC-0030 NGEO-WEBC-VTC-0110 NGEO-WEBC-VTC-0150</t>
   </si>
   <si>
@@ -1305,9 +1302,6 @@
   </si>
   <si>
     <t>NGEO-WEBC-VTC-0110 NGEO-WEBC-VTC-0120</t>
-  </si>
-  <si>
-    <t>NGEO-WEBC-VTC-0120 NGEO-WEBC-VTC-0121 NGEO-WEBC-VTC-0122</t>
   </si>
   <si>
     <t>NGEO-WEBC-VTC-0130 NGEO-WEBC-VTC-0131 NGEO-WEBC-VTC-0140</t>
@@ -1443,6 +1437,12 @@
   </si>
   <si>
     <t xml:space="preserve">ngEO-SUB-050-WEBC-DES  ngEO-SUB-159-WEBC-FUN  ngEO-SUB-163-WEBC-FUN  ngEO-SUB-164-WEBC-FUN  </t>
+  </si>
+  <si>
+    <t> NGEO-WEBC-VTC-0120 NGEO-WEBC-VTC-0125 NGEO-WEBC-VTC-0126</t>
+  </si>
+  <si>
+    <t>NGEO-WEBC-VTC-0120 NGEO-WEBC-VTC-0125 NGEO-WEBC-VTC-0126</t>
   </si>
 </sst>
 </file>
@@ -1607,7 +1607,7 @@
 </file>
 
 <file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
-<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{C5A4FDCC-B057-486F-A690-4CF3495032D1}" diskRevisions="1" revisionId="169" version="17">
+<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{1AAA0089-E698-48A5-A82E-0104D36DE94F}" diskRevisions="1" revisionId="171" version="18">
   <header guid="{4F90D1E1-98D7-43D2-BD00-631CFD24DD58}" dateTime="2012-11-30T15:11:14" maxSheetId="4" userName="Emna Mokaddem" r:id="rId1">
     <sheetIdMap count="3">
       <sheetId val="1"/>
@@ -1727,6 +1727,13 @@
       <sheetId val="3"/>
     </sheetIdMap>
   </header>
+  <header guid="{1AAA0089-E698-48A5-A82E-0104D36DE94F}" dateTime="2012-12-20T18:36:38" maxSheetId="4" userName="Emna Mokaddem" r:id="rId18" minRId="170" maxRId="171">
+    <sheetIdMap count="3">
+      <sheetId val="1"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+    </sheetIdMap>
+  </header>
 </headers>
 </file>
 
@@ -5707,6 +5714,35 @@
 </revisions>
 </file>
 
+<file path=xl/revisions/revisionLog18.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="170" sId="1">
+    <oc r="D36" t="inlineStr">
+      <is>
+        <t> NGEO-WEBC-VTC-0120 NGEO-WEBC-VTC-0121 NGEO-WEBC-VTC-0122</t>
+      </is>
+    </oc>
+    <nc r="D36" t="inlineStr">
+      <is>
+        <t> NGEO-WEBC-VTC-0120 NGEO-WEBC-VTC-0125 NGEO-WEBC-VTC-0126</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="171" sId="1">
+    <oc r="D100" t="inlineStr">
+      <is>
+        <t>NGEO-WEBC-VTC-0120 NGEO-WEBC-VTC-0121 NGEO-WEBC-VTC-0122</t>
+      </is>
+    </oc>
+    <nc r="D100" t="inlineStr">
+      <is>
+        <t>NGEO-WEBC-VTC-0120 NGEO-WEBC-VTC-0125 NGEO-WEBC-VTC-0126</t>
+      </is>
+    </nc>
+  </rcc>
+</revisions>
+</file>
+
 <file path=xl/revisions/revisionLog2.xml><?xml version="1.0" encoding="utf-8"?>
 <revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <rcc rId="1" sId="1" xfDxf="1" dxf="1">
@@ -6021,9 +6057,10 @@
 </file>
 
 <file path=xl/revisions/userNames.xml><?xml version="1.0" encoding="utf-8"?>
-<users xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" count="2">
+<users xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" count="3">
   <userInfo guid="{A8C1A900-A0EB-4515-8E78-8138C0C42F21}" name="Emna Mokaddem" id="-2083828105" dateTime="2012-11-30T15:11:14"/>
   <userInfo guid="{BFC4EE2A-90DF-4511-9F1D-C131A45F9081}" name="Emna Mokaddem" id="-2083842149" dateTime="2012-12-10T10:19:06"/>
+  <userInfo guid="{1AAA0089-E698-48A5-A82E-0104D36DE94F}" name="Emna Mokaddem" id="-2083845639" dateTime="2012-12-20T18:35:37"/>
 </users>
 </file>
 
@@ -6314,11 +6351,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:D191"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C196" sqref="C196"/>
+    <sheetView tabSelected="1" topLeftCell="A175" workbookViewId="0">
+      <selection activeCell="D190" sqref="D190"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6343,7 +6379,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" s="8" customFormat="1" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" s="8" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
         <v>4</v>
       </c>
@@ -6357,7 +6393,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="21" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>8</v>
       </c>
@@ -6371,7 +6407,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>10</v>
       </c>
@@ -6383,7 +6419,7 @@
       </c>
       <c r="D4" s="6"/>
     </row>
-    <row r="5" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>12</v>
       </c>
@@ -6395,7 +6431,7 @@
       </c>
       <c r="D5" s="6"/>
     </row>
-    <row r="6" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>14</v>
       </c>
@@ -6407,7 +6443,7 @@
       </c>
       <c r="D6" s="6"/>
     </row>
-    <row r="7" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
         <v>16</v>
       </c>
@@ -6419,7 +6455,7 @@
       </c>
       <c r="D7" s="6"/>
     </row>
-    <row r="8" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
         <v>18</v>
       </c>
@@ -6431,7 +6467,7 @@
       </c>
       <c r="D8" s="6"/>
     </row>
-    <row r="9" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
         <v>20</v>
       </c>
@@ -6445,7 +6481,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
         <v>22</v>
       </c>
@@ -6457,7 +6493,7 @@
       </c>
       <c r="D10" s="6"/>
     </row>
-    <row r="11" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
         <v>24</v>
       </c>
@@ -6469,7 +6505,7 @@
       </c>
       <c r="D11" s="6"/>
     </row>
-    <row r="12" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
         <v>27</v>
       </c>
@@ -6481,7 +6517,7 @@
       </c>
       <c r="D12" s="6"/>
     </row>
-    <row r="13" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="5" t="s">
         <v>29</v>
       </c>
@@ -6495,7 +6531,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
         <v>31</v>
       </c>
@@ -6507,7 +6543,7 @@
       </c>
       <c r="D14" s="6"/>
     </row>
-    <row r="15" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="s">
         <v>33</v>
       </c>
@@ -6519,7 +6555,7 @@
       </c>
       <c r="D15" s="6"/>
     </row>
-    <row r="16" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="5" t="s">
         <v>35</v>
       </c>
@@ -6531,7 +6567,7 @@
       </c>
       <c r="D16" s="6"/>
     </row>
-    <row r="17" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="5" t="s">
         <v>37</v>
       </c>
@@ -6543,7 +6579,7 @@
       </c>
       <c r="D17" s="6"/>
     </row>
-    <row r="18" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="5" t="s">
         <v>39</v>
       </c>
@@ -6555,7 +6591,7 @@
       </c>
       <c r="D18" s="6"/>
     </row>
-    <row r="19" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="6" t="s">
         <v>41</v>
       </c>
@@ -6569,7 +6605,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="6" t="s">
         <v>44</v>
       </c>
@@ -6581,7 +6617,7 @@
       </c>
       <c r="D20" s="6"/>
     </row>
-    <row r="21" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="5" t="s">
         <v>46</v>
       </c>
@@ -6595,7 +6631,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="6" t="s">
         <v>48</v>
       </c>
@@ -6609,7 +6645,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="6" t="s">
         <v>52</v>
       </c>
@@ -6620,10 +6656,10 @@
         <v>50</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>449</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="5" t="s">
         <v>54</v>
       </c>
@@ -6637,7 +6673,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="5" t="s">
         <v>56</v>
       </c>
@@ -6660,10 +6696,10 @@
         <v>26</v>
       </c>
       <c r="D26" s="6" t="s">
-        <v>450</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="5" t="s">
         <v>60</v>
       </c>
@@ -6675,7 +6711,7 @@
       </c>
       <c r="D27" s="6"/>
     </row>
-    <row r="28" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="5" t="s">
         <v>62</v>
       </c>
@@ -6687,7 +6723,7 @@
       </c>
       <c r="D28" s="6"/>
     </row>
-    <row r="29" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="5" t="s">
         <v>64</v>
       </c>
@@ -6699,7 +6735,7 @@
       </c>
       <c r="D29" s="6"/>
     </row>
-    <row r="30" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="5" t="s">
         <v>66</v>
       </c>
@@ -6711,7 +6747,7 @@
       </c>
       <c r="D30" s="6"/>
     </row>
-    <row r="31" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="5" t="s">
         <v>68</v>
       </c>
@@ -6723,7 +6759,7 @@
       </c>
       <c r="D31" s="6"/>
     </row>
-    <row r="32" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="5" t="s">
         <v>70</v>
       </c>
@@ -6735,7 +6771,7 @@
       </c>
       <c r="D32" s="6"/>
     </row>
-    <row r="33" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="5" t="s">
         <v>72</v>
       </c>
@@ -6747,7 +6783,7 @@
       </c>
       <c r="D33" s="6"/>
     </row>
-    <row r="34" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="5" t="s">
         <v>74</v>
       </c>
@@ -6759,7 +6795,7 @@
       </c>
       <c r="D34" s="6"/>
     </row>
-    <row r="35" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="5" t="s">
         <v>76</v>
       </c>
@@ -6771,7 +6807,7 @@
       </c>
       <c r="D35" s="6"/>
     </row>
-    <row r="36" spans="1:4" ht="23.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="5" t="s">
         <v>78</v>
       </c>
@@ -6782,10 +6818,10 @@
         <v>26</v>
       </c>
       <c r="D36" s="6" t="s">
-        <v>410</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="5" t="s">
         <v>80</v>
       </c>
@@ -6797,7 +6833,7 @@
       </c>
       <c r="D37" s="6"/>
     </row>
-    <row r="38" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="5" t="s">
         <v>82</v>
       </c>
@@ -6809,7 +6845,7 @@
       </c>
       <c r="D38" s="6"/>
     </row>
-    <row r="39" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="5" t="s">
         <v>84</v>
       </c>
@@ -6821,7 +6857,7 @@
       </c>
       <c r="D39" s="6"/>
     </row>
-    <row r="40" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="5" t="s">
         <v>86</v>
       </c>
@@ -6833,7 +6869,7 @@
       </c>
       <c r="D40" s="6"/>
     </row>
-    <row r="41" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="5" t="s">
         <v>88</v>
       </c>
@@ -6845,7 +6881,7 @@
       </c>
       <c r="D41" s="6"/>
     </row>
-    <row r="42" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="5" t="s">
         <v>90</v>
       </c>
@@ -6857,7 +6893,7 @@
       </c>
       <c r="D42" s="6"/>
     </row>
-    <row r="43" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="5" t="s">
         <v>92</v>
       </c>
@@ -6880,10 +6916,10 @@
         <v>50</v>
       </c>
       <c r="D44" s="6" t="s">
-        <v>411</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="5" t="s">
         <v>97</v>
       </c>
@@ -6897,7 +6933,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="46" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="5" t="s">
         <v>100</v>
       </c>
@@ -6911,7 +6947,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="47" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="5" t="s">
         <v>102</v>
       </c>
@@ -6925,7 +6961,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="48" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="5" t="s">
         <v>104</v>
       </c>
@@ -6936,10 +6972,10 @@
         <v>50</v>
       </c>
       <c r="D48" s="6" t="s">
-        <v>449</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" s="5" t="s">
         <v>106</v>
       </c>
@@ -6950,10 +6986,10 @@
         <v>50</v>
       </c>
       <c r="D49" s="6" t="s">
-        <v>455</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" s="5" t="s">
         <v>108</v>
       </c>
@@ -6965,7 +7001,7 @@
       </c>
       <c r="D50" s="6"/>
     </row>
-    <row r="51" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="5" t="s">
         <v>110</v>
       </c>
@@ -6976,10 +7012,10 @@
         <v>50</v>
       </c>
       <c r="D51" s="6" t="s">
-        <v>455</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52" s="5" t="s">
         <v>112</v>
       </c>
@@ -6990,10 +7026,10 @@
         <v>50</v>
       </c>
       <c r="D52" s="6" t="s">
-        <v>449</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A53" s="5" t="s">
         <v>114</v>
       </c>
@@ -7007,7 +7043,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="54" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A54" s="5" t="s">
         <v>116</v>
       </c>
@@ -7021,7 +7057,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="55" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A55" s="5" t="s">
         <v>117</v>
       </c>
@@ -7035,7 +7071,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="56" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A56" s="5" t="s">
         <v>119</v>
       </c>
@@ -7049,7 +7085,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="57" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A57" s="5" t="s">
         <v>121</v>
       </c>
@@ -7063,7 +7099,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="58" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A58" s="5" t="s">
         <v>123</v>
       </c>
@@ -7075,7 +7111,7 @@
       </c>
       <c r="D58" s="6"/>
     </row>
-    <row r="59" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A59" s="5" t="s">
         <v>125</v>
       </c>
@@ -7087,7 +7123,7 @@
       </c>
       <c r="D59" s="6"/>
     </row>
-    <row r="60" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A60" s="5" t="s">
         <v>127</v>
       </c>
@@ -7099,7 +7135,7 @@
       </c>
       <c r="D60" s="6"/>
     </row>
-    <row r="61" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A61" s="5" t="s">
         <v>129</v>
       </c>
@@ -7111,7 +7147,7 @@
       </c>
       <c r="D61" s="6"/>
     </row>
-    <row r="62" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A62" s="5" t="s">
         <v>131</v>
       </c>
@@ -7123,7 +7159,7 @@
       </c>
       <c r="D62" s="6"/>
     </row>
-    <row r="63" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A63" s="5" t="s">
         <v>133</v>
       </c>
@@ -7135,7 +7171,7 @@
       </c>
       <c r="D63" s="6"/>
     </row>
-    <row r="64" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A64" s="5" t="s">
         <v>135</v>
       </c>
@@ -7147,7 +7183,7 @@
       </c>
       <c r="D64" s="6"/>
     </row>
-    <row r="65" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A65" s="5" t="s">
         <v>136</v>
       </c>
@@ -7161,7 +7197,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="66" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A66" s="5" t="s">
         <v>139</v>
       </c>
@@ -7173,7 +7209,7 @@
       </c>
       <c r="D66" s="6"/>
     </row>
-    <row r="67" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A67" s="5" t="s">
         <v>141</v>
       </c>
@@ -7187,7 +7223,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="68" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A68" s="5" t="s">
         <v>143</v>
       </c>
@@ -7199,7 +7235,7 @@
       </c>
       <c r="D68" s="6"/>
     </row>
-    <row r="69" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A69" s="5" t="s">
         <v>145</v>
       </c>
@@ -7211,7 +7247,7 @@
       </c>
       <c r="D69" s="6"/>
     </row>
-    <row r="70" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A70" s="5" t="s">
         <v>147</v>
       </c>
@@ -7223,7 +7259,7 @@
       </c>
       <c r="D70" s="6"/>
     </row>
-    <row r="71" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A71" s="5" t="s">
         <v>149</v>
       </c>
@@ -7237,7 +7273,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="72" spans="1:4" ht="23.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:4" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A72" s="5" t="s">
         <v>151</v>
       </c>
@@ -7249,7 +7285,7 @@
       </c>
       <c r="D72" s="6"/>
     </row>
-    <row r="73" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A73" s="5" t="s">
         <v>153</v>
       </c>
@@ -7261,7 +7297,7 @@
       </c>
       <c r="D73" s="6"/>
     </row>
-    <row r="74" spans="1:4" ht="23.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:4" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A74" s="5" t="s">
         <v>155</v>
       </c>
@@ -7273,7 +7309,7 @@
       </c>
       <c r="D74" s="6"/>
     </row>
-    <row r="75" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A75" s="5" t="s">
         <v>157</v>
       </c>
@@ -7285,7 +7321,7 @@
       </c>
       <c r="D75" s="6"/>
     </row>
-    <row r="76" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A76" s="5" t="s">
         <v>159</v>
       </c>
@@ -7299,7 +7335,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="77" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A77" s="5" t="s">
         <v>161</v>
       </c>
@@ -7311,7 +7347,7 @@
       </c>
       <c r="D77" s="6"/>
     </row>
-    <row r="78" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A78" s="5" t="s">
         <v>163</v>
       </c>
@@ -7325,7 +7361,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="79" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A79" s="5" t="s">
         <v>164</v>
       </c>
@@ -7339,7 +7375,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="80" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A80" s="5" t="s">
         <v>166</v>
       </c>
@@ -7351,7 +7387,7 @@
       </c>
       <c r="D80" s="6"/>
     </row>
-    <row r="81" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A81" s="5" t="s">
         <v>168</v>
       </c>
@@ -7365,7 +7401,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="82" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A82" s="5" t="s">
         <v>170</v>
       </c>
@@ -7377,7 +7413,7 @@
       </c>
       <c r="D82" s="6"/>
     </row>
-    <row r="83" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A83" s="5" t="s">
         <v>171</v>
       </c>
@@ -7389,7 +7425,7 @@
       </c>
       <c r="D83" s="6"/>
     </row>
-    <row r="84" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A84" s="5" t="s">
         <v>173</v>
       </c>
@@ -7401,7 +7437,7 @@
       </c>
       <c r="D84" s="6"/>
     </row>
-    <row r="85" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A85" s="5" t="s">
         <v>174</v>
       </c>
@@ -7413,7 +7449,7 @@
       </c>
       <c r="D85" s="6"/>
     </row>
-    <row r="86" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A86" s="5" t="s">
         <v>175</v>
       </c>
@@ -7425,7 +7461,7 @@
       </c>
       <c r="D86" s="6"/>
     </row>
-    <row r="87" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A87" s="5" t="s">
         <v>177</v>
       </c>
@@ -7437,7 +7473,7 @@
       </c>
       <c r="D87" s="6"/>
     </row>
-    <row r="88" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A88" s="5" t="s">
         <v>179</v>
       </c>
@@ -7449,7 +7485,7 @@
       </c>
       <c r="D88" s="6"/>
     </row>
-    <row r="89" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A89" s="5" t="s">
         <v>181</v>
       </c>
@@ -7463,7 +7499,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="90" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A90" s="5" t="s">
         <v>183</v>
       </c>
@@ -7475,7 +7511,7 @@
       </c>
       <c r="D90" s="6"/>
     </row>
-    <row r="91" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A91" s="5" t="s">
         <v>184</v>
       </c>
@@ -7487,7 +7523,7 @@
       </c>
       <c r="D91" s="6"/>
     </row>
-    <row r="92" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A92" s="5" t="s">
         <v>186</v>
       </c>
@@ -7499,7 +7535,7 @@
       </c>
       <c r="D92" s="6"/>
     </row>
-    <row r="93" spans="1:4" ht="23.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:4" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A93" s="5" t="s">
         <v>188</v>
       </c>
@@ -7510,7 +7546,7 @@
         <v>50</v>
       </c>
       <c r="D93" s="6" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="94" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -7524,10 +7560,10 @@
         <v>50</v>
       </c>
       <c r="D94" s="6" t="s">
-        <v>413</v>
-      </c>
-    </row>
-    <row r="95" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A95" s="5" t="s">
         <v>192</v>
       </c>
@@ -7538,10 +7574,10 @@
         <v>50</v>
       </c>
       <c r="D95" s="6" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="96" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A96" s="5" t="s">
         <v>194</v>
       </c>
@@ -7555,7 +7591,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="97" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A97" s="5" t="s">
         <v>196</v>
       </c>
@@ -7567,7 +7603,7 @@
       </c>
       <c r="D97" s="6"/>
     </row>
-    <row r="98" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A98" s="5" t="s">
         <v>198</v>
       </c>
@@ -7579,7 +7615,7 @@
       </c>
       <c r="D98" s="6"/>
     </row>
-    <row r="99" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A99" s="5" t="s">
         <v>200</v>
       </c>
@@ -7593,7 +7629,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="100" spans="1:4" ht="23.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:4" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A100" s="5" t="s">
         <v>202</v>
       </c>
@@ -7604,10 +7640,10 @@
         <v>50</v>
       </c>
       <c r="D100" s="6" t="s">
-        <v>415</v>
-      </c>
-    </row>
-    <row r="101" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A101" s="5" t="s">
         <v>204</v>
       </c>
@@ -7618,10 +7654,10 @@
         <v>50</v>
       </c>
       <c r="D101" s="6" t="s">
-        <v>412</v>
-      </c>
-    </row>
-    <row r="102" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A102" s="5" t="s">
         <v>206</v>
       </c>
@@ -7633,7 +7669,7 @@
       </c>
       <c r="D102" s="6"/>
     </row>
-    <row r="103" spans="1:4" ht="23.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:4" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A103" s="5" t="s">
         <v>208</v>
       </c>
@@ -7644,10 +7680,10 @@
         <v>50</v>
       </c>
       <c r="D103" s="6" t="s">
-        <v>412</v>
-      </c>
-    </row>
-    <row r="104" spans="1:4" ht="23.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A104" s="5" t="s">
         <v>210</v>
       </c>
@@ -7658,10 +7694,10 @@
         <v>50</v>
       </c>
       <c r="D104" s="6" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="105" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A105" s="5" t="s">
         <v>212</v>
       </c>
@@ -7675,7 +7711,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="106" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A106" s="5" t="s">
         <v>214</v>
       </c>
@@ -7689,7 +7725,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="107" spans="1:4" ht="23.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:4" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A107" s="5" t="s">
         <v>216</v>
       </c>
@@ -7700,10 +7736,10 @@
         <v>50</v>
       </c>
       <c r="D107" s="6" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="108" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A108" s="5" t="s">
         <v>218</v>
       </c>
@@ -7715,7 +7751,7 @@
       </c>
       <c r="D108" s="6"/>
     </row>
-    <row r="109" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A109" s="5" t="s">
         <v>220</v>
       </c>
@@ -7727,7 +7763,7 @@
       </c>
       <c r="D109" s="6"/>
     </row>
-    <row r="110" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A110" s="5" t="s">
         <v>222</v>
       </c>
@@ -7739,7 +7775,7 @@
       </c>
       <c r="D110" s="6"/>
     </row>
-    <row r="111" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A111" s="5" t="s">
         <v>224</v>
       </c>
@@ -7751,7 +7787,7 @@
       </c>
       <c r="D111" s="6"/>
     </row>
-    <row r="112" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A112" s="5" t="s">
         <v>226</v>
       </c>
@@ -7763,7 +7799,7 @@
       </c>
       <c r="D112" s="6"/>
     </row>
-    <row r="113" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A113" s="5" t="s">
         <v>228</v>
       </c>
@@ -7775,7 +7811,7 @@
       </c>
       <c r="D113" s="6"/>
     </row>
-    <row r="114" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A114" s="5" t="s">
         <v>230</v>
       </c>
@@ -7787,7 +7823,7 @@
       </c>
       <c r="D114" s="6"/>
     </row>
-    <row r="115" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A115" s="5" t="s">
         <v>232</v>
       </c>
@@ -7799,7 +7835,7 @@
       </c>
       <c r="D115" s="6"/>
     </row>
-    <row r="116" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A116" s="5" t="s">
         <v>234</v>
       </c>
@@ -7811,7 +7847,7 @@
       </c>
       <c r="D116" s="6"/>
     </row>
-    <row r="117" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A117" s="5" t="s">
         <v>236</v>
       </c>
@@ -7823,7 +7859,7 @@
       </c>
       <c r="D117" s="6"/>
     </row>
-    <row r="118" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A118" s="5" t="s">
         <v>238</v>
       </c>
@@ -7835,7 +7871,7 @@
       </c>
       <c r="D118" s="6"/>
     </row>
-    <row r="119" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A119" s="5" t="s">
         <v>240</v>
       </c>
@@ -7847,7 +7883,7 @@
       </c>
       <c r="D119" s="6"/>
     </row>
-    <row r="120" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A120" s="5" t="s">
         <v>242</v>
       </c>
@@ -7859,7 +7895,7 @@
       </c>
       <c r="D120" s="6"/>
     </row>
-    <row r="121" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A121" s="5" t="s">
         <v>244</v>
       </c>
@@ -7871,7 +7907,7 @@
       </c>
       <c r="D121" s="6"/>
     </row>
-    <row r="122" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A122" s="5" t="s">
         <v>246</v>
       </c>
@@ -7883,7 +7919,7 @@
       </c>
       <c r="D122" s="6"/>
     </row>
-    <row r="123" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A123" s="5" t="s">
         <v>248</v>
       </c>
@@ -7895,7 +7931,7 @@
       </c>
       <c r="D123" s="6"/>
     </row>
-    <row r="124" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A124" s="5" t="s">
         <v>250</v>
       </c>
@@ -7907,7 +7943,7 @@
       </c>
       <c r="D124" s="6"/>
     </row>
-    <row r="125" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A125" s="5" t="s">
         <v>252</v>
       </c>
@@ -7919,7 +7955,7 @@
       </c>
       <c r="D125" s="6"/>
     </row>
-    <row r="126" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A126" s="5" t="s">
         <v>254</v>
       </c>
@@ -7931,7 +7967,7 @@
       </c>
       <c r="D126" s="6"/>
     </row>
-    <row r="127" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A127" s="5" t="s">
         <v>256</v>
       </c>
@@ -7943,7 +7979,7 @@
       </c>
       <c r="D127" s="6"/>
     </row>
-    <row r="128" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A128" s="5" t="s">
         <v>258</v>
       </c>
@@ -7955,7 +7991,7 @@
       </c>
       <c r="D128" s="6"/>
     </row>
-    <row r="129" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A129" s="5" t="s">
         <v>260</v>
       </c>
@@ -7967,7 +8003,7 @@
       </c>
       <c r="D129" s="6"/>
     </row>
-    <row r="130" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A130" s="5" t="s">
         <v>262</v>
       </c>
@@ -7979,7 +8015,7 @@
       </c>
       <c r="D130" s="6"/>
     </row>
-    <row r="131" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A131" s="5" t="s">
         <v>264</v>
       </c>
@@ -7993,7 +8029,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="132" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A132" s="5" t="s">
         <v>266</v>
       </c>
@@ -8005,7 +8041,7 @@
       </c>
       <c r="D132" s="6"/>
     </row>
-    <row r="133" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A133" s="5" t="s">
         <v>268</v>
       </c>
@@ -8017,7 +8053,7 @@
       </c>
       <c r="D133" s="6"/>
     </row>
-    <row r="134" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A134" s="5" t="s">
         <v>270</v>
       </c>
@@ -8029,7 +8065,7 @@
       </c>
       <c r="D134" s="6"/>
     </row>
-    <row r="135" spans="1:4" ht="23.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:4" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A135" s="5" t="s">
         <v>272</v>
       </c>
@@ -8041,7 +8077,7 @@
       </c>
       <c r="D135" s="6"/>
     </row>
-    <row r="136" spans="1:4" ht="23.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:4" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A136" s="5" t="s">
         <v>274</v>
       </c>
@@ -8053,7 +8089,7 @@
       </c>
       <c r="D136" s="6"/>
     </row>
-    <row r="137" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A137" s="5" t="s">
         <v>276</v>
       </c>
@@ -8065,7 +8101,7 @@
       </c>
       <c r="D137" s="6"/>
     </row>
-    <row r="138" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A138" s="5" t="s">
         <v>278</v>
       </c>
@@ -8077,7 +8113,7 @@
       </c>
       <c r="D138" s="6"/>
     </row>
-    <row r="139" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A139" s="5" t="s">
         <v>280</v>
       </c>
@@ -8089,7 +8125,7 @@
       </c>
       <c r="D139" s="6"/>
     </row>
-    <row r="140" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A140" s="5" t="s">
         <v>282</v>
       </c>
@@ -8101,7 +8137,7 @@
       </c>
       <c r="D140" s="6"/>
     </row>
-    <row r="141" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A141" s="5" t="s">
         <v>284</v>
       </c>
@@ -8115,7 +8151,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="142" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A142" s="5" t="s">
         <v>286</v>
       </c>
@@ -8129,7 +8165,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="143" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A143" s="5" t="s">
         <v>288</v>
       </c>
@@ -8143,7 +8179,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="144" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A144" s="5" t="s">
         <v>290</v>
       </c>
@@ -8155,7 +8191,7 @@
       </c>
       <c r="D144" s="6"/>
     </row>
-    <row r="145" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A145" s="5" t="s">
         <v>292</v>
       </c>
@@ -8169,7 +8205,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="146" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A146" s="5" t="s">
         <v>294</v>
       </c>
@@ -8183,7 +8219,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="147" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A147" s="5" t="s">
         <v>296</v>
       </c>
@@ -8208,10 +8244,10 @@
         <v>6</v>
       </c>
       <c r="D148" s="6" t="s">
-        <v>417</v>
-      </c>
-    </row>
-    <row r="149" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="149" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A149" s="5" t="s">
         <v>300</v>
       </c>
@@ -8223,7 +8259,7 @@
       </c>
       <c r="D149" s="6"/>
     </row>
-    <row r="150" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A150" s="5" t="s">
         <v>302</v>
       </c>
@@ -8235,7 +8271,7 @@
       </c>
       <c r="D150" s="6"/>
     </row>
-    <row r="151" spans="1:4" ht="23.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:4" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A151" s="5" t="s">
         <v>304</v>
       </c>
@@ -8249,7 +8285,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="152" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A152" s="5" t="s">
         <v>306</v>
       </c>
@@ -8261,7 +8297,7 @@
       </c>
       <c r="D152" s="6"/>
     </row>
-    <row r="153" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A153" s="5" t="s">
         <v>308</v>
       </c>
@@ -8273,7 +8309,7 @@
       </c>
       <c r="D153" s="6"/>
     </row>
-    <row r="154" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A154" s="5" t="s">
         <v>310</v>
       </c>
@@ -8285,7 +8321,7 @@
       </c>
       <c r="D154" s="6"/>
     </row>
-    <row r="155" spans="1:4" ht="23.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:4" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A155" s="5" t="s">
         <v>312</v>
       </c>
@@ -8296,10 +8332,10 @@
         <v>6</v>
       </c>
       <c r="D155" s="6" t="s">
-        <v>418</v>
-      </c>
-    </row>
-    <row r="156" spans="1:4" ht="23.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="156" spans="1:4" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A156" s="5" t="s">
         <v>314</v>
       </c>
@@ -8313,7 +8349,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="157" spans="1:4" ht="23.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:4" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A157" s="5" t="s">
         <v>316</v>
       </c>
@@ -8327,7 +8363,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="158" spans="1:4" ht="23.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:4" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A158" s="5" t="s">
         <v>318</v>
       </c>
@@ -8339,7 +8375,7 @@
       </c>
       <c r="D158" s="6"/>
     </row>
-    <row r="159" spans="1:4" ht="23.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:4" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A159" s="5" t="s">
         <v>320</v>
       </c>
@@ -8351,7 +8387,7 @@
       </c>
       <c r="D159" s="6"/>
     </row>
-    <row r="160" spans="1:4" ht="23.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:4" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A160" s="5" t="s">
         <v>322</v>
       </c>
@@ -8363,7 +8399,7 @@
       </c>
       <c r="D160" s="6"/>
     </row>
-    <row r="161" spans="1:4" ht="23.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:4" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A161" s="5" t="s">
         <v>324</v>
       </c>
@@ -8375,7 +8411,7 @@
       </c>
       <c r="D161" s="6"/>
     </row>
-    <row r="162" spans="1:4" ht="23.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:4" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A162" s="5" t="s">
         <v>326</v>
       </c>
@@ -8389,7 +8425,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="163" spans="1:4" ht="23.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:4" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A163" s="5" t="s">
         <v>328</v>
       </c>
@@ -8401,7 +8437,7 @@
       </c>
       <c r="D163" s="6"/>
     </row>
-    <row r="164" spans="1:4" ht="23.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:4" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A164" s="5" t="s">
         <v>330</v>
       </c>
@@ -8415,7 +8451,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="165" spans="1:4" ht="23.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:4" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A165" s="5" t="s">
         <v>332</v>
       </c>
@@ -8426,10 +8462,10 @@
         <v>26</v>
       </c>
       <c r="D165" s="6" t="s">
-        <v>419</v>
-      </c>
-    </row>
-    <row r="166" spans="1:4" ht="23.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="166" spans="1:4" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A166" s="5" t="s">
         <v>334</v>
       </c>
@@ -8441,7 +8477,7 @@
       </c>
       <c r="D166" s="6"/>
     </row>
-    <row r="167" spans="1:4" ht="23.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:4" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A167" s="5" t="s">
         <v>336</v>
       </c>
@@ -8453,7 +8489,7 @@
       </c>
       <c r="D167" s="6"/>
     </row>
-    <row r="168" spans="1:4" ht="23.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:4" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A168" s="5" t="s">
         <v>338</v>
       </c>
@@ -8467,7 +8503,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="169" spans="1:4" ht="23.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:4" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A169" s="5" t="s">
         <v>340</v>
       </c>
@@ -8479,7 +8515,7 @@
       </c>
       <c r="D169" s="6"/>
     </row>
-    <row r="170" spans="1:4" ht="23.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:4" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A170" s="5" t="s">
         <v>342</v>
       </c>
@@ -8491,7 +8527,7 @@
       </c>
       <c r="D170" s="6"/>
     </row>
-    <row r="171" spans="1:4" ht="23.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:4" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A171" s="5" t="s">
         <v>344</v>
       </c>
@@ -8503,7 +8539,7 @@
       </c>
       <c r="D171" s="6"/>
     </row>
-    <row r="172" spans="1:4" ht="23.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:4" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A172" s="5" t="s">
         <v>346</v>
       </c>
@@ -8515,7 +8551,7 @@
       </c>
       <c r="D172" s="6"/>
     </row>
-    <row r="173" spans="1:4" ht="23.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:4" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A173" s="5" t="s">
         <v>348</v>
       </c>
@@ -8527,7 +8563,7 @@
       </c>
       <c r="D173" s="6"/>
     </row>
-    <row r="174" spans="1:4" ht="23.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:4" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A174" s="5" t="s">
         <v>350</v>
       </c>
@@ -8539,7 +8575,7 @@
       </c>
       <c r="D174" s="6"/>
     </row>
-    <row r="175" spans="1:4" ht="23.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:4" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A175" s="5" t="s">
         <v>352</v>
       </c>
@@ -8551,7 +8587,7 @@
       </c>
       <c r="D175" s="6"/>
     </row>
-    <row r="176" spans="1:4" ht="23.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:4" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A176" s="5" t="s">
         <v>354</v>
       </c>
@@ -8565,7 +8601,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="177" spans="1:4" ht="23.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:4" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A177" s="5" t="s">
         <v>356</v>
       </c>
@@ -8577,7 +8613,7 @@
       </c>
       <c r="D177" s="6"/>
     </row>
-    <row r="178" spans="1:4" ht="23.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:4" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A178" s="5" t="s">
         <v>358</v>
       </c>
@@ -8589,7 +8625,7 @@
       </c>
       <c r="D178" s="6"/>
     </row>
-    <row r="179" spans="1:4" ht="23.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:4" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A179" s="5" t="s">
         <v>360</v>
       </c>
@@ -8601,7 +8637,7 @@
       </c>
       <c r="D179" s="6"/>
     </row>
-    <row r="180" spans="1:4" ht="23.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:4" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A180" s="5" t="s">
         <v>362</v>
       </c>
@@ -8613,7 +8649,7 @@
       </c>
       <c r="D180" s="6"/>
     </row>
-    <row r="181" spans="1:4" ht="23.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:4" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A181" s="5" t="s">
         <v>364</v>
       </c>
@@ -8625,7 +8661,7 @@
       </c>
       <c r="D181" s="6"/>
     </row>
-    <row r="182" spans="1:4" ht="23.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:4" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A182" s="5" t="s">
         <v>366</v>
       </c>
@@ -8639,7 +8675,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="183" spans="1:4" ht="23.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:4" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A183" s="5" t="s">
         <v>368</v>
       </c>
@@ -8653,7 +8689,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="184" spans="1:4" ht="23.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:4" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A184" s="5" t="s">
         <v>370</v>
       </c>
@@ -8664,7 +8700,7 @@
         <v>50</v>
       </c>
       <c r="D184" s="6" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
     </row>
     <row r="185" spans="1:4" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -8678,10 +8714,10 @@
         <v>50</v>
       </c>
       <c r="D185" s="6" t="s">
-        <v>417</v>
-      </c>
-    </row>
-    <row r="186" spans="1:4" ht="23.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="186" spans="1:4" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A186" s="5" t="s">
         <v>374</v>
       </c>
@@ -8692,10 +8728,10 @@
         <v>50</v>
       </c>
       <c r="D186" s="6" t="s">
-        <v>412</v>
-      </c>
-    </row>
-    <row r="187" spans="1:4" ht="23.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="187" spans="1:4" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A187" s="5" t="s">
         <v>376</v>
       </c>
@@ -8706,10 +8742,10 @@
         <v>50</v>
       </c>
       <c r="D187" s="6" t="s">
-        <v>420</v>
-      </c>
-    </row>
-    <row r="188" spans="1:4" ht="23.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="188" spans="1:4" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A188" s="5" t="s">
         <v>378</v>
       </c>
@@ -8721,7 +8757,7 @@
       </c>
       <c r="D188" s="6"/>
     </row>
-    <row r="189" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A189" s="5" t="s">
         <v>380</v>
       </c>
@@ -8733,7 +8769,7 @@
       </c>
       <c r="D189" s="6"/>
     </row>
-    <row r="190" spans="1:4" ht="23.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:4" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A190" s="5" t="s">
         <v>382</v>
       </c>
@@ -8747,7 +8783,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="191" spans="1:4" ht="23.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:4" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A191" s="5" t="s">
         <v>384</v>
       </c>
@@ -8762,25 +8798,16 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:D191">
-    <filterColumn colId="3">
-      <filters>
-        <filter val="NGEO-WEBC-VTC-0030 NGEO-WEBC-VTC-0110 NGEO-WEBC-VTC-0150"/>
-        <filter val="NGEO-WEBC-VTC-0150"/>
-        <filter val="NGEO-WEBC-VTC-0150  NGEO-WEBC-VTC-0151"/>
-        <filter val="NGEO-WEBC-VTC-0150 NGEO-WEBC-VTC-0151"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:D191"/>
   <customSheetViews>
-    <customSheetView guid="{DA65F8B0-9E28-4694-AD16-567217749021}" showAutoFilter="1" topLeftCell="A112">
-      <selection activeCell="A141" sqref="A141"/>
+    <customSheetView guid="{62558FE4-8837-4E09-B150-242C582E08A1}" showAutoFilter="1" topLeftCell="A4">
+      <selection activeCell="D10" sqref="D10"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
       <autoFilter ref="A1:D191"/>
     </customSheetView>
-    <customSheetView guid="{62558FE4-8837-4E09-B150-242C582E08A1}" showAutoFilter="1" topLeftCell="A4">
-      <selection activeCell="D10" sqref="D10"/>
+    <customSheetView guid="{DA65F8B0-9E28-4694-AD16-567217749021}" showAutoFilter="1" topLeftCell="A112">
+      <selection activeCell="A141" sqref="A141"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
       <autoFilter ref="A1:D191"/>
@@ -8796,8 +8823,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8820,73 +8847,73 @@
     </row>
     <row r="2" spans="1:3" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>393</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>394</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>395</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="34.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="B5" s="6" t="s">
         <v>396</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="34.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="B6" s="6" t="s">
         <v>397</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="34.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="B7" s="6" t="s">
         <v>398</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="B8" s="6" t="s">
         <v>399</v>
@@ -8897,105 +8924,104 @@
     </row>
     <row r="9" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="B9" s="6" t="s">
         <v>400</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
+        <v>429</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>430</v>
+      </c>
+      <c r="C11" s="6" t="s">
         <v>431</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>432</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>433</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="5" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
+        <v>436</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>437</v>
+      </c>
+      <c r="C14" s="6" t="s">
         <v>438</v>
-      </c>
-      <c r="B14" s="6" t="s">
-        <v>439</v>
-      </c>
-      <c r="C14" s="6" t="s">
-        <v>440</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="5" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
     </row>
   </sheetData>
   <customSheetViews>
+    <customSheetView guid="{62558FE4-8837-4E09-B150-242C582E08A1}">
+      <selection activeCell="C29" sqref="C29"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+    </customSheetView>
     <customSheetView guid="{DA65F8B0-9E28-4694-AD16-567217749021}">
       <selection activeCell="E8" sqref="E8"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
-    <customSheetView guid="{62558FE4-8837-4E09-B150-242C582E08A1}">
-      <selection activeCell="C29" sqref="C29"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-    </customSheetView>
   </customSheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -9115,11 +9141,11 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{DA65F8B0-9E28-4694-AD16-567217749021}">
+    <customSheetView guid="{62558FE4-8837-4E09-B150-242C582E08A1}">
       <selection activeCell="C16" sqref="C16"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
-    <customSheetView guid="{62558FE4-8837-4E09-B150-242C582E08A1}">
+    <customSheetView guid="{DA65F8B0-9E28-4694-AD16-567217749021}">
       <selection activeCell="C16" sqref="C16"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>

</xml_diff>

<commit_message>
Update SSTP with validation tests for Help and import
</commit_message>
<xml_diff>
--- a/documentation/Req_SSTP.xlsx
+++ b/documentation/Req_SSTP.xlsx
@@ -1608,13 +1608,6 @@
 
 <file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
 <headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{1AAA0089-E698-48A5-A82E-0104D36DE94F}" diskRevisions="1" revisionId="171" version="18">
-  <header guid="{4F90D1E1-98D7-43D2-BD00-631CFD24DD58}" dateTime="2012-11-30T15:11:14" maxSheetId="4" userName="Emna Mokaddem" r:id="rId1">
-    <sheetIdMap count="3">
-      <sheetId val="1"/>
-      <sheetId val="2"/>
-      <sheetId val="3"/>
-    </sheetIdMap>
-  </header>
   <header guid="{A8C1A900-A0EB-4515-8E78-8138C0C42F21}" dateTime="2012-11-30T15:17:24" maxSheetId="4" userName="Emna Mokaddem" r:id="rId2" minRId="1" maxRId="5">
     <sheetIdMap count="3">
       <sheetId val="1"/>
@@ -1735,10 +1728,6 @@
     </sheetIdMap>
   </header>
 </headers>
-</file>
-
-<file path=xl/revisions/revisionLog1.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac"/>
 </file>
 
 <file path=xl/revisions/revisionLog10.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>